<commit_message>
Inclusion of CSP technologies
</commit_message>
<xml_diff>
--- a/Base/Data/Inputs/Data_ammonia_paper.xlsx
+++ b/Base/Data/Inputs/Data_ammonia_paper.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7380" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6180"/>
   </bookViews>
   <sheets>
     <sheet name="Data_base_case" sheetId="79" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="173">
   <si>
     <t>Red: Don't change the name without changing the Julia code</t>
   </si>
@@ -434,9 +434,6 @@
     <t>Fixed cost (EUR/Capacity installed/y)</t>
   </si>
   <si>
-    <t>Variable cost (EUR/Output)</t>
-  </si>
-  <si>
     <t>Fuel selling price (EUR/output)</t>
   </si>
   <si>
@@ -558,6 +555,9 @@
   </si>
   <si>
     <t>Reactant3</t>
+  </si>
+  <si>
+    <t>Variable cost (EUR/output)</t>
   </si>
 </sst>
 </file>
@@ -773,7 +773,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="132">
+  <cellXfs count="130">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -813,7 +813,6 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1010,9 +1009,6 @@
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1902,11 +1898,11 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Y36"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="5" topLeftCell="I6" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="5" ySplit="5" topLeftCell="W6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
-      <selection pane="bottomRight" activeCell="F6" sqref="F6"/>
+      <selection pane="bottomRight" activeCell="Z1" sqref="Z1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1919,7 +1915,7 @@
     <col min="6" max="6" width="11.453125" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="28.90625" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.7265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.453125" style="115" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.453125" style="113" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.36328125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.7265625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
@@ -1939,156 +1935,175 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="123" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="123"/>
-      <c r="C1" s="123"/>
-      <c r="D1" s="123"/>
-      <c r="E1" s="124"/>
-      <c r="F1" s="45" t="s">
+      <c r="A1" s="121" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="121"/>
+      <c r="C1" s="121"/>
+      <c r="D1" s="121"/>
+      <c r="E1" s="122"/>
+      <c r="F1" s="44" t="s">
         <v>99</v>
       </c>
-      <c r="G1" s="45" t="s">
+      <c r="G1" s="44" t="s">
         <v>106</v>
       </c>
-      <c r="H1" s="46" t="s">
+      <c r="H1" s="45" t="s">
         <v>65</v>
       </c>
-      <c r="I1" s="111" t="s">
+      <c r="I1" s="110" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="46" t="s">
+      <c r="J1" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="46" t="s">
+      <c r="K1" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="47" t="s">
+      <c r="L1" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="M1" s="46" t="s">
+      <c r="M1" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="N1" s="48" t="s">
+      <c r="N1" s="47" t="s">
         <v>66</v>
       </c>
-      <c r="O1" s="48" t="s">
+      <c r="O1" s="47" t="s">
         <v>67</v>
       </c>
-      <c r="P1" s="48" t="s">
+      <c r="P1" s="47" t="s">
         <v>68</v>
       </c>
-      <c r="Q1" s="48" t="s">
+      <c r="Q1" s="47" t="s">
         <v>69</v>
       </c>
-      <c r="R1" s="48" t="s">
+      <c r="R1" s="47" t="s">
         <v>70</v>
       </c>
-      <c r="S1" s="48" t="s">
+      <c r="S1" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="T1" s="48" t="s">
+      <c r="T1" s="47" t="s">
         <v>129</v>
       </c>
-      <c r="U1" s="48" t="s">
+      <c r="U1" s="47" t="s">
         <v>130</v>
       </c>
-      <c r="V1" s="48" t="s">
+      <c r="V1" s="47" t="s">
+        <v>172</v>
+      </c>
+      <c r="W1" s="47" t="s">
         <v>131</v>
       </c>
-      <c r="W1" s="48" t="s">
+      <c r="X1" s="47" t="s">
         <v>132</v>
       </c>
-      <c r="X1" s="48" t="s">
-        <v>133</v>
-      </c>
-      <c r="Y1" s="51" t="s">
+      <c r="Y1" s="50" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:25" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="33"/>
-      <c r="B2" s="126" t="s">
+      <c r="A2" s="32"/>
+      <c r="B2" s="124" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="127" t="s">
+      <c r="C2" s="125" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="126" t="s">
+      <c r="D2" s="124" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="35" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="18" t="s">
-        <v>99</v>
+      <c r="E2" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="18" t="str">
+        <f>F1</f>
+        <v>Used (1 or 0)</v>
       </c>
       <c r="G2" s="18" t="str">
-        <f>G1</f>
+        <f t="shared" ref="G2:Y2" si="0">G1</f>
         <v>Unit tag</v>
       </c>
-      <c r="H2" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="I2" s="112" t="s">
-        <v>2</v>
-      </c>
-      <c r="J2" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="K2" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="L2" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="M2" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="N2" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="O2" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="P2" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q2" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="R2" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="S2" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="T2" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="U2" s="19" t="s">
-        <v>130</v>
-      </c>
-      <c r="V2" s="19" t="s">
-        <v>131</v>
-      </c>
-      <c r="W2" s="19" t="s">
-        <v>132</v>
-      </c>
-      <c r="X2" s="19" t="s">
-        <v>133</v>
-      </c>
-      <c r="Y2" s="19" t="s">
-        <v>72</v>
+      <c r="H2" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>Yearly demand (kg fuel)</v>
+      </c>
+      <c r="I2" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>Produced from</v>
+      </c>
+      <c r="J2" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>El balance</v>
+      </c>
+      <c r="K2" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>Heat balance</v>
+      </c>
+      <c r="L2" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>H2 balance</v>
+      </c>
+      <c r="M2" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>Max Capacity</v>
+      </c>
+      <c r="N2" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>Fuel production rate (kg output/kg input)</v>
+      </c>
+      <c r="O2" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>Heat generated (kWh/output)</v>
+      </c>
+      <c r="P2" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>Load min (% of max capacity)</v>
+      </c>
+      <c r="Q2" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>Ramp up (% of capacity /h)</v>
+      </c>
+      <c r="R2" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>Ramp down (% of capacity /h)</v>
+      </c>
+      <c r="S2" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>Electrical consumption (kWh/output)</v>
+      </c>
+      <c r="T2" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>Investment (EUR/Capacity installed)</v>
+      </c>
+      <c r="U2" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>Fixed cost (EUR/Capacity installed/y)</v>
+      </c>
+      <c r="V2" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>Variable cost (EUR/output)</v>
+      </c>
+      <c r="W2" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>Fuel selling price (EUR/output)</v>
+      </c>
+      <c r="X2" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>Fuel buying price (EUR/output)</v>
+      </c>
+      <c r="Y2" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>Annuity factor</v>
       </c>
     </row>
     <row r="3" spans="1:25" s="6" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="34"/>
-      <c r="B3" s="126"/>
-      <c r="C3" s="127"/>
-      <c r="D3" s="126"/>
-      <c r="E3" s="35" t="s">
+      <c r="A3" s="33"/>
+      <c r="B3" s="124"/>
+      <c r="C3" s="125"/>
+      <c r="D3" s="124"/>
+      <c r="E3" s="34" t="s">
         <v>80</v>
       </c>
       <c r="F3" s="15" t="s">
@@ -2100,7 +2115,7 @@
       <c r="H3" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="I3" s="113" t="s">
+      <c r="I3" s="111" t="s">
         <v>100</v>
       </c>
       <c r="J3" s="15" t="s">
@@ -2115,49 +2130,49 @@
       <c r="M3" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="N3" s="49">
+      <c r="N3" s="48">
         <v>2020</v>
       </c>
-      <c r="O3" s="120">
+      <c r="O3" s="118">
         <v>2020</v>
       </c>
-      <c r="P3" s="120">
+      <c r="P3" s="118">
         <v>2020</v>
       </c>
-      <c r="Q3" s="120">
+      <c r="Q3" s="118">
         <v>2020</v>
       </c>
-      <c r="R3" s="120">
+      <c r="R3" s="118">
         <v>2020</v>
       </c>
-      <c r="S3" s="120">
+      <c r="S3" s="118">
         <v>2020</v>
       </c>
-      <c r="T3" s="120">
+      <c r="T3" s="118">
         <v>2020</v>
       </c>
-      <c r="U3" s="120">
+      <c r="U3" s="118">
         <v>2020</v>
       </c>
-      <c r="V3" s="120">
+      <c r="V3" s="118">
         <v>2020</v>
       </c>
-      <c r="W3" s="120">
+      <c r="W3" s="118">
         <v>2020</v>
       </c>
-      <c r="X3" s="120">
+      <c r="X3" s="118">
         <v>2020</v>
       </c>
-      <c r="Y3" s="120">
+      <c r="Y3" s="118">
         <v>2020</v>
       </c>
     </row>
     <row r="4" spans="1:25" s="6" customFormat="1" ht="4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="34"/>
-      <c r="B4" s="126"/>
-      <c r="C4" s="127"/>
-      <c r="D4" s="126"/>
-      <c r="E4" s="35"/>
+      <c r="A4" s="33"/>
+      <c r="B4" s="124"/>
+      <c r="C4" s="125"/>
+      <c r="D4" s="124"/>
+      <c r="E4" s="34"/>
       <c r="F4" s="15" t="str">
         <f>F2&amp;F3</f>
         <v>Used (1 or 0)All</v>
@@ -2167,106 +2182,106 @@
         <v>Unit tagAll</v>
       </c>
       <c r="H4" s="15" t="str">
-        <f t="shared" ref="H4:M4" si="0">H2&amp;H3</f>
+        <f t="shared" ref="H4:M4" si="1">H2&amp;H3</f>
         <v>Yearly demand (kg fuel)All</v>
       </c>
-      <c r="I4" s="113" t="str">
-        <f t="shared" si="0"/>
+      <c r="I4" s="111" t="str">
+        <f t="shared" si="1"/>
         <v>Produced fromAll</v>
       </c>
       <c r="J4" s="15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>El balanceAll</v>
       </c>
       <c r="K4" s="15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Heat balanceAll</v>
       </c>
       <c r="L4" s="15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>H2 balanceAll</v>
       </c>
       <c r="M4" s="15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Max CapacityAll</v>
       </c>
       <c r="N4" s="15" t="str">
-        <f t="shared" ref="N4:S4" si="1">N2&amp;N3</f>
+        <f t="shared" ref="N4:S4" si="2">N2&amp;N3</f>
         <v>Fuel production rate (kg output/kg input)2020</v>
       </c>
       <c r="O4" s="15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Heat generated (kWh/output)2020</v>
       </c>
       <c r="P4" s="15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Load min (% of max capacity)2020</v>
       </c>
       <c r="Q4" s="15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Ramp up (% of capacity /h)2020</v>
       </c>
       <c r="R4" s="15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Ramp down (% of capacity /h)2020</v>
       </c>
       <c r="S4" s="15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Electrical consumption (kWh/output)2020</v>
       </c>
       <c r="T4" s="15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="U4" s="15" t="str">
-        <f t="shared" ref="U4:Y4" si="2">U2&amp;U3</f>
+        <f t="shared" ref="U4:Y4" si="3">U2&amp;U3</f>
         <v>Fixed cost (EUR/Capacity installed/y)2020</v>
       </c>
       <c r="V4" s="15" t="str">
-        <f t="shared" si="2"/>
-        <v>Variable cost (EUR/Output)2020</v>
+        <f t="shared" si="3"/>
+        <v>Variable cost (EUR/output)2020</v>
       </c>
       <c r="W4" s="15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Fuel selling price (EUR/output)2020</v>
       </c>
       <c r="X4" s="15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Fuel buying price (EUR/output)2020</v>
       </c>
       <c r="Y4" s="15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Annuity factor2020</v>
       </c>
     </row>
     <row r="5" spans="1:25" s="8" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="126"/>
-      <c r="C5" s="127"/>
-      <c r="D5" s="126"/>
-      <c r="E5" s="50" t="s">
+      <c r="B5" s="124"/>
+      <c r="C5" s="125"/>
+      <c r="D5" s="124"/>
+      <c r="E5" s="49" t="s">
         <v>10</v>
       </c>
       <c r="F5" s="8">
-        <f t="shared" ref="F5:M5" si="3">COLUMN(F2)-COLUMN($E$5)</f>
+        <f t="shared" ref="F5:M5" si="4">COLUMN(F2)-COLUMN($E$5)</f>
         <v>1</v>
       </c>
       <c r="G5" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="H5" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
-      <c r="I5" s="114">
-        <f t="shared" si="3"/>
+      <c r="I5" s="112">
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="J5" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="K5" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="L5" s="8">
@@ -2274,241 +2289,241 @@
         <v>7</v>
       </c>
       <c r="M5" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="N5" s="8">
-        <f t="shared" ref="N5:S5" si="4">COLUMN(N2)-COLUMN($E$5)</f>
+        <f t="shared" ref="N5:S5" si="5">COLUMN(N2)-COLUMN($E$5)</f>
         <v>9</v>
       </c>
       <c r="O5" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="P5" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>11</v>
       </c>
       <c r="Q5" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>12</v>
       </c>
       <c r="R5" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>13</v>
       </c>
       <c r="S5" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>14</v>
       </c>
       <c r="T5" s="8">
         <v>17</v>
       </c>
       <c r="U5" s="8">
-        <f t="shared" ref="U5:Y5" si="5">COLUMN(U2)-COLUMN($E$5)</f>
+        <f t="shared" ref="U5:Y5" si="6">COLUMN(U2)-COLUMN($E$5)</f>
         <v>16</v>
       </c>
       <c r="V5" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>17</v>
       </c>
       <c r="W5" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>18</v>
       </c>
       <c r="X5" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>19</v>
       </c>
       <c r="Y5" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:25" s="70" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="122" t="s">
+    <row r="6" spans="1:25" s="69" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="120" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="65" t="s">
+      <c r="B6" s="64" t="s">
         <v>101</v>
       </c>
-      <c r="C6" s="66" t="s">
+      <c r="C6" s="65" t="s">
         <v>123</v>
       </c>
-      <c r="D6" s="67" t="s">
-        <v>157</v>
+      <c r="D6" s="66" t="s">
+        <v>156</v>
       </c>
       <c r="E6" s="9">
-        <f t="shared" ref="E6:E36" si="6">ROW(D6)-ROW($E$5)</f>
-        <v>1</v>
-      </c>
-      <c r="F6" s="68">
-        <v>1</v>
-      </c>
-      <c r="G6" s="68" t="s">
+        <f t="shared" ref="E6:E36" si="7">ROW(D6)-ROW($E$5)</f>
+        <v>1</v>
+      </c>
+      <c r="F6" s="67">
+        <v>1</v>
+      </c>
+      <c r="G6" s="67" t="s">
         <v>74</v>
       </c>
-      <c r="H6" s="70">
+      <c r="H6" s="69">
         <f>430*10^6</f>
         <v>430000000</v>
       </c>
-      <c r="I6" s="69" t="str">
+      <c r="I6" s="68" t="str">
         <f>B11</f>
         <v>Reactant3</v>
       </c>
-      <c r="J6" s="70">
-        <v>0</v>
-      </c>
-      <c r="K6" s="70">
-        <v>1</v>
-      </c>
-      <c r="L6" s="70">
-        <v>0</v>
-      </c>
-      <c r="M6" s="70">
+      <c r="J6" s="69">
+        <v>0</v>
+      </c>
+      <c r="K6" s="69">
+        <v>1</v>
+      </c>
+      <c r="L6" s="69">
+        <v>0</v>
+      </c>
+      <c r="M6" s="69">
         <v>20000</v>
       </c>
-      <c r="N6" s="106">
+      <c r="N6" s="105">
         <v>5.2910052910052912</v>
       </c>
-      <c r="O6" s="70">
-        <v>0</v>
-      </c>
-      <c r="P6" s="71">
+      <c r="O6" s="69">
+        <v>0</v>
+      </c>
+      <c r="P6" s="70">
         <v>0.4</v>
       </c>
-      <c r="Q6" s="71">
+      <c r="Q6" s="70">
         <v>0.2</v>
       </c>
-      <c r="R6" s="70">
+      <c r="R6" s="69">
         <v>0.2</v>
       </c>
-      <c r="S6" s="70">
+      <c r="S6" s="69">
         <v>0.38</v>
       </c>
-      <c r="T6" s="70">
+      <c r="T6" s="69">
         <v>4192</v>
       </c>
-      <c r="U6" s="70">
+      <c r="U6" s="69">
         <v>436</v>
       </c>
-      <c r="V6" s="70">
-        <v>0</v>
-      </c>
-      <c r="W6" s="70">
-        <v>0</v>
-      </c>
-      <c r="X6" s="78">
-        <v>0</v>
-      </c>
-      <c r="Y6" s="70">
+      <c r="V6" s="69">
+        <v>0</v>
+      </c>
+      <c r="W6" s="69">
+        <v>0</v>
+      </c>
+      <c r="X6" s="77">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="69">
         <v>9.3678779051968114E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:25" s="70" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="122"/>
-      <c r="B7" s="65" t="s">
+    <row r="7" spans="1:25" s="69" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="120"/>
+      <c r="B7" s="64" t="s">
         <v>101</v>
       </c>
-      <c r="C7" s="66" t="s">
+      <c r="C7" s="65" t="s">
         <v>123</v>
       </c>
-      <c r="D7" s="67" t="s">
-        <v>158</v>
+      <c r="D7" s="66" t="s">
+        <v>157</v>
       </c>
       <c r="E7" s="9">
         <f>ROW(D7)-ROW($E$5)</f>
         <v>2</v>
       </c>
-      <c r="F7" s="68">
-        <v>1</v>
-      </c>
-      <c r="G7" s="68" t="s">
+      <c r="F7" s="67">
+        <v>1</v>
+      </c>
+      <c r="G7" s="67" t="s">
         <v>75</v>
       </c>
-      <c r="H7" s="70">
+      <c r="H7" s="69">
         <f>430*10^6</f>
         <v>430000000</v>
       </c>
-      <c r="I7" s="69" t="str">
+      <c r="I7" s="68" t="str">
         <f>B11</f>
         <v>Reactant3</v>
       </c>
-      <c r="J7" s="70">
-        <v>0</v>
-      </c>
-      <c r="K7" s="70">
-        <v>1</v>
-      </c>
-      <c r="L7" s="70">
-        <v>0</v>
-      </c>
-      <c r="M7" s="70">
+      <c r="J7" s="69">
+        <v>0</v>
+      </c>
+      <c r="K7" s="69">
+        <v>1</v>
+      </c>
+      <c r="L7" s="69">
+        <v>0</v>
+      </c>
+      <c r="M7" s="69">
         <f>M6</f>
         <v>20000</v>
       </c>
-      <c r="N7" s="106">
+      <c r="N7" s="105">
         <v>5.2910052910052912</v>
       </c>
-      <c r="O7" s="70">
-        <v>0</v>
-      </c>
-      <c r="P7" s="71">
+      <c r="O7" s="69">
+        <v>0</v>
+      </c>
+      <c r="P7" s="70">
         <v>0.4</v>
       </c>
-      <c r="Q7" s="71">
+      <c r="Q7" s="70">
         <v>0.2</v>
       </c>
-      <c r="R7" s="70">
+      <c r="R7" s="69">
         <v>0.2</v>
       </c>
-      <c r="S7" s="70">
+      <c r="S7" s="69">
         <v>0.83</v>
       </c>
-      <c r="T7" s="70">
+      <c r="T7" s="69">
         <v>4192</v>
       </c>
-      <c r="U7" s="70">
+      <c r="U7" s="69">
         <v>828</v>
       </c>
-      <c r="V7" s="70">
-        <v>0</v>
-      </c>
-      <c r="W7" s="70">
-        <v>0</v>
-      </c>
-      <c r="X7" s="78">
-        <v>0</v>
-      </c>
-      <c r="Y7" s="70">
+      <c r="V7" s="69">
+        <v>0</v>
+      </c>
+      <c r="W7" s="69">
+        <v>0</v>
+      </c>
+      <c r="X7" s="77">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="69">
         <v>9.3678779051968114E-2</v>
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A8" s="122"/>
-      <c r="B8" s="20" t="s">
-        <v>170</v>
+      <c r="A8" s="120"/>
+      <c r="B8" s="19" t="s">
+        <v>169</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>150</v>
-      </c>
-      <c r="D8" s="56" t="s">
-        <v>153</v>
+        <v>149</v>
+      </c>
+      <c r="D8" s="55" t="s">
+        <v>152</v>
       </c>
       <c r="E8" s="9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="F8" s="2">
         <v>1</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H8">
         <v>0</v>
       </c>
-      <c r="I8" s="115" t="s">
+      <c r="I8" s="113" t="s">
         <v>12</v>
       </c>
       <c r="J8">
@@ -2560,713 +2575,713 @@
         <v>0.10185220882315059</v>
       </c>
     </row>
-    <row r="9" spans="1:25" s="83" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="122"/>
-      <c r="B9" s="79" t="s">
-        <v>171</v>
-      </c>
-      <c r="C9" s="80" t="s">
-        <v>150</v>
-      </c>
-      <c r="D9" s="81" t="s">
-        <v>143</v>
+    <row r="9" spans="1:25" s="82" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="120"/>
+      <c r="B9" s="78" t="s">
+        <v>170</v>
+      </c>
+      <c r="C9" s="79" t="s">
+        <v>149</v>
+      </c>
+      <c r="D9" s="80" t="s">
+        <v>142</v>
       </c>
       <c r="E9" s="9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
-      <c r="F9" s="82">
-        <v>1</v>
-      </c>
-      <c r="G9" s="82" t="s">
+      <c r="F9" s="81">
+        <v>1</v>
+      </c>
+      <c r="G9" s="81" t="s">
         <v>76</v>
       </c>
-      <c r="H9" s="83">
-        <v>0</v>
-      </c>
-      <c r="I9" s="84" t="str">
+      <c r="H9" s="82">
+        <v>0</v>
+      </c>
+      <c r="I9" s="83" t="str">
         <f>B8</f>
         <v>Reactant1</v>
       </c>
-      <c r="J9" s="83">
-        <v>0</v>
-      </c>
-      <c r="K9" s="83">
-        <v>1</v>
-      </c>
-      <c r="L9" s="83">
-        <v>1</v>
-      </c>
-      <c r="M9" s="83">
+      <c r="J9" s="82">
+        <v>0</v>
+      </c>
+      <c r="K9" s="82">
+        <v>1</v>
+      </c>
+      <c r="L9" s="82">
+        <v>1</v>
+      </c>
+      <c r="M9" s="82">
         <v>20000</v>
       </c>
-      <c r="N9" s="83">
+      <c r="N9" s="82">
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="O9" s="83">
+      <c r="O9" s="82">
         <v>7.07</v>
       </c>
-      <c r="P9" s="85">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="85">
-        <v>1</v>
-      </c>
-      <c r="R9" s="83">
-        <v>1</v>
-      </c>
-      <c r="S9" s="83">
+      <c r="P9" s="84">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="84">
+        <v>1</v>
+      </c>
+      <c r="R9" s="82">
+        <v>1</v>
+      </c>
+      <c r="S9" s="82">
         <v>51.5</v>
       </c>
-      <c r="T9" s="83">
+      <c r="T9" s="82">
         <v>56467</v>
       </c>
-      <c r="U9" s="83">
+      <c r="U9" s="82">
         <v>1129</v>
       </c>
-      <c r="V9" s="83">
-        <v>0</v>
-      </c>
-      <c r="W9" s="83">
-        <v>0</v>
-      </c>
-      <c r="X9" s="86">
-        <v>0</v>
-      </c>
-      <c r="Y9" s="83">
+      <c r="V9" s="82">
+        <v>0</v>
+      </c>
+      <c r="W9" s="82">
+        <v>0</v>
+      </c>
+      <c r="X9" s="85">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="82">
         <v>9.3678779051968114E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:25" s="91" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="122"/>
-      <c r="B10" s="87" t="s">
-        <v>171</v>
-      </c>
-      <c r="C10" s="88" t="s">
-        <v>150</v>
-      </c>
-      <c r="D10" s="89" t="s">
+    <row r="10" spans="1:25" s="90" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="120"/>
+      <c r="B10" s="86" t="s">
+        <v>170</v>
+      </c>
+      <c r="C10" s="87" t="s">
+        <v>149</v>
+      </c>
+      <c r="D10" s="88" t="s">
+        <v>145</v>
+      </c>
+      <c r="E10" s="9">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="F10" s="89">
+        <v>1</v>
+      </c>
+      <c r="G10" s="89" t="s">
         <v>146</v>
       </c>
-      <c r="E10" s="9">
-        <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="F10" s="90">
-        <v>1</v>
-      </c>
-      <c r="G10" s="90" t="s">
-        <v>147</v>
-      </c>
-      <c r="H10" s="91">
-        <v>0</v>
-      </c>
-      <c r="I10" s="92" t="str">
+      <c r="H10" s="90">
+        <v>0</v>
+      </c>
+      <c r="I10" s="91" t="str">
         <f>B8</f>
         <v>Reactant1</v>
       </c>
-      <c r="J10" s="91">
-        <v>0</v>
-      </c>
-      <c r="K10" s="91">
-        <v>1</v>
-      </c>
-      <c r="L10" s="91">
-        <v>1</v>
-      </c>
-      <c r="M10" s="91">
+      <c r="J10" s="90">
+        <v>0</v>
+      </c>
+      <c r="K10" s="90">
+        <v>1</v>
+      </c>
+      <c r="L10" s="90">
+        <v>1</v>
+      </c>
+      <c r="M10" s="90">
         <f>M9</f>
         <v>20000</v>
       </c>
-      <c r="N10" s="91">
+      <c r="N10" s="90">
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="O10" s="91">
-        <v>0</v>
-      </c>
-      <c r="P10" s="93">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="93">
-        <v>1</v>
-      </c>
-      <c r="R10" s="94">
-        <v>1</v>
-      </c>
-      <c r="S10" s="94">
+      <c r="O10" s="90">
+        <v>0</v>
+      </c>
+      <c r="P10" s="92">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="92">
+        <v>1</v>
+      </c>
+      <c r="R10" s="93">
+        <v>1</v>
+      </c>
+      <c r="S10" s="93">
         <v>37.9</v>
       </c>
-      <c r="T10" s="94">
+      <c r="T10" s="93">
         <v>131493</v>
       </c>
-      <c r="U10" s="91">
+      <c r="U10" s="90">
         <v>3945</v>
       </c>
-      <c r="V10" s="91">
-        <v>0</v>
-      </c>
-      <c r="W10" s="91">
-        <v>0</v>
-      </c>
-      <c r="X10" s="95">
-        <v>0</v>
-      </c>
-      <c r="Y10" s="91">
+      <c r="V10" s="90">
+        <v>0</v>
+      </c>
+      <c r="W10" s="90">
+        <v>0</v>
+      </c>
+      <c r="X10" s="94">
+        <v>0</v>
+      </c>
+      <c r="Y10" s="90">
         <v>9.3678779051968114E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:25" s="58" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="122"/>
-      <c r="B11" s="107" t="s">
-        <v>172</v>
-      </c>
-      <c r="C11" s="108" t="s">
-        <v>150</v>
-      </c>
-      <c r="D11" s="56" t="s">
+    <row r="11" spans="1:25" s="57" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="120"/>
+      <c r="B11" s="106" t="s">
+        <v>171</v>
+      </c>
+      <c r="C11" s="107" t="s">
+        <v>149</v>
+      </c>
+      <c r="D11" s="55" t="s">
         <v>29</v>
       </c>
       <c r="E11" s="9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>6</v>
       </c>
-      <c r="F11" s="109">
-        <v>1</v>
-      </c>
-      <c r="G11" s="109" t="s">
+      <c r="F11" s="108">
+        <v>1</v>
+      </c>
+      <c r="G11" s="108" t="s">
         <v>18</v>
       </c>
-      <c r="H11" s="44">
-        <v>0</v>
-      </c>
-      <c r="I11" s="116" t="s">
+      <c r="H11" s="43">
+        <v>0</v>
+      </c>
+      <c r="I11" s="114" t="s">
         <v>12</v>
       </c>
-      <c r="J11" s="58">
-        <v>0</v>
-      </c>
-      <c r="K11" s="58">
-        <v>0</v>
-      </c>
-      <c r="L11" s="58">
+      <c r="J11" s="57">
+        <v>0</v>
+      </c>
+      <c r="K11" s="57">
+        <v>0</v>
+      </c>
+      <c r="L11" s="57">
         <v>-1</v>
       </c>
-      <c r="M11" s="58">
+      <c r="M11" s="57">
         <f>M9</f>
         <v>20000</v>
       </c>
-      <c r="N11" s="44">
-        <v>0</v>
-      </c>
-      <c r="O11" s="58">
-        <v>0</v>
-      </c>
-      <c r="P11" s="110">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="110">
-        <v>1</v>
-      </c>
-      <c r="R11" s="44">
-        <v>1</v>
-      </c>
-      <c r="S11" s="44">
-        <v>0</v>
-      </c>
-      <c r="T11" s="44">
-        <v>0</v>
-      </c>
-      <c r="U11" s="44">
-        <v>0</v>
-      </c>
-      <c r="V11" s="44">
-        <v>0</v>
-      </c>
-      <c r="W11" s="44">
-        <v>0</v>
-      </c>
-      <c r="X11" s="44">
-        <v>0</v>
-      </c>
-      <c r="Y11" s="58">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:25" s="43" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="122"/>
-      <c r="B12" s="72" t="s">
+      <c r="N11" s="43">
+        <v>0</v>
+      </c>
+      <c r="O11" s="57">
+        <v>0</v>
+      </c>
+      <c r="P11" s="109">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="109">
+        <v>1</v>
+      </c>
+      <c r="R11" s="43">
+        <v>1</v>
+      </c>
+      <c r="S11" s="43">
+        <v>0</v>
+      </c>
+      <c r="T11" s="43">
+        <v>0</v>
+      </c>
+      <c r="U11" s="43">
+        <v>0</v>
+      </c>
+      <c r="V11" s="43">
+        <v>0</v>
+      </c>
+      <c r="W11" s="43">
+        <v>0</v>
+      </c>
+      <c r="X11" s="43">
+        <v>0</v>
+      </c>
+      <c r="Y11" s="57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" s="42" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="120"/>
+      <c r="B12" s="71" t="s">
         <v>101</v>
       </c>
-      <c r="C12" s="121" t="s">
-        <v>167</v>
-      </c>
-      <c r="D12" s="74" t="s">
+      <c r="C12" s="119" t="s">
+        <v>166</v>
+      </c>
+      <c r="D12" s="73" t="s">
         <v>32</v>
       </c>
       <c r="E12" s="9">
         <f>ROW(D12)-ROW($E$5)</f>
         <v>7</v>
       </c>
-      <c r="F12" s="75">
-        <v>1</v>
-      </c>
-      <c r="G12" s="75" t="s">
+      <c r="F12" s="74">
+        <v>1</v>
+      </c>
+      <c r="G12" s="74" t="s">
         <v>13</v>
       </c>
-      <c r="H12" s="43">
-        <v>0</v>
-      </c>
-      <c r="I12" s="76" t="str">
+      <c r="H12" s="42">
+        <v>0</v>
+      </c>
+      <c r="I12" s="75" t="str">
         <f>B9</f>
         <v>Product/Reactant2</v>
       </c>
-      <c r="J12" s="43">
-        <v>0</v>
-      </c>
-      <c r="K12" s="43">
-        <v>0</v>
-      </c>
-      <c r="L12" s="43">
-        <v>0</v>
-      </c>
-      <c r="M12" s="43">
+      <c r="J12" s="42">
+        <v>0</v>
+      </c>
+      <c r="K12" s="42">
+        <v>0</v>
+      </c>
+      <c r="L12" s="42">
+        <v>0</v>
+      </c>
+      <c r="M12" s="42">
         <f>9*M9</f>
         <v>180000</v>
       </c>
-      <c r="N12" s="43">
+      <c r="N12" s="42">
         <v>7.76</v>
       </c>
-      <c r="O12" s="43">
-        <v>0</v>
-      </c>
-      <c r="P12" s="77">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="77">
-        <v>1</v>
-      </c>
-      <c r="R12" s="43">
-        <v>1</v>
-      </c>
-      <c r="S12" s="43">
-        <v>0</v>
-      </c>
-      <c r="T12" s="43">
-        <v>0</v>
-      </c>
-      <c r="U12" s="43">
-        <v>0</v>
-      </c>
-      <c r="V12" s="43">
-        <v>0</v>
-      </c>
-      <c r="W12" s="43">
+      <c r="O12" s="42">
+        <v>0</v>
+      </c>
+      <c r="P12" s="76">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="76">
+        <v>1</v>
+      </c>
+      <c r="R12" s="42">
+        <v>1</v>
+      </c>
+      <c r="S12" s="42">
+        <v>0</v>
+      </c>
+      <c r="T12" s="42">
+        <v>0</v>
+      </c>
+      <c r="U12" s="42">
+        <v>0</v>
+      </c>
+      <c r="V12" s="42">
+        <v>0</v>
+      </c>
+      <c r="W12" s="42">
         <v>0.05</v>
       </c>
-      <c r="X12" s="43">
-        <v>0</v>
-      </c>
-      <c r="Y12" s="43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:25" s="43" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="122"/>
-      <c r="B13" s="72" t="s">
+      <c r="X12" s="42">
+        <v>0</v>
+      </c>
+      <c r="Y12" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" s="42" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="120"/>
+      <c r="B13" s="71" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="73" t="s">
-        <v>150</v>
-      </c>
-      <c r="D13" s="74" t="s">
+      <c r="C13" s="72" t="s">
+        <v>149</v>
+      </c>
+      <c r="D13" s="73" t="s">
         <v>30</v>
       </c>
       <c r="E13" s="9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
-      <c r="F13" s="75">
-        <v>1</v>
-      </c>
-      <c r="G13" s="75" t="s">
+      <c r="F13" s="74">
+        <v>1</v>
+      </c>
+      <c r="G13" s="74" t="s">
         <v>19</v>
       </c>
-      <c r="H13" s="96">
-        <v>0</v>
-      </c>
-      <c r="I13" s="76" t="s">
+      <c r="H13" s="95">
+        <v>0</v>
+      </c>
+      <c r="I13" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="J13" s="43">
-        <v>0</v>
-      </c>
-      <c r="K13" s="43">
-        <v>1</v>
-      </c>
-      <c r="L13" s="43">
-        <v>0</v>
-      </c>
-      <c r="M13" s="43">
+      <c r="J13" s="42">
+        <v>0</v>
+      </c>
+      <c r="K13" s="42">
+        <v>1</v>
+      </c>
+      <c r="L13" s="42">
+        <v>0</v>
+      </c>
+      <c r="M13" s="42">
         <f>M18</f>
         <v>2000000</v>
       </c>
-      <c r="N13" s="96">
-        <v>0</v>
-      </c>
-      <c r="O13" s="43">
-        <v>0</v>
-      </c>
-      <c r="P13" s="77">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="77">
-        <v>1</v>
-      </c>
-      <c r="R13" s="96">
-        <v>1</v>
-      </c>
-      <c r="S13" s="96">
-        <v>0</v>
-      </c>
-      <c r="T13" s="96">
-        <v>0</v>
-      </c>
-      <c r="U13" s="96">
-        <v>0</v>
-      </c>
-      <c r="V13" s="96">
-        <v>0</v>
-      </c>
-      <c r="W13" s="96">
-        <v>0</v>
-      </c>
-      <c r="X13" s="96">
-        <v>0</v>
-      </c>
-      <c r="Y13" s="43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:25" s="43" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="122"/>
-      <c r="B14" s="72" t="s">
+      <c r="N13" s="95">
+        <v>0</v>
+      </c>
+      <c r="O13" s="42">
+        <v>0</v>
+      </c>
+      <c r="P13" s="76">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="76">
+        <v>1</v>
+      </c>
+      <c r="R13" s="95">
+        <v>1</v>
+      </c>
+      <c r="S13" s="95">
+        <v>0</v>
+      </c>
+      <c r="T13" s="95">
+        <v>0</v>
+      </c>
+      <c r="U13" s="95">
+        <v>0</v>
+      </c>
+      <c r="V13" s="95">
+        <v>0</v>
+      </c>
+      <c r="W13" s="95">
+        <v>0</v>
+      </c>
+      <c r="X13" s="95">
+        <v>0</v>
+      </c>
+      <c r="Y13" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" s="42" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="120"/>
+      <c r="B14" s="71" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="121" t="s">
-        <v>168</v>
-      </c>
-      <c r="D14" s="74" t="s">
+      <c r="C14" s="119" t="s">
+        <v>167</v>
+      </c>
+      <c r="D14" s="73" t="s">
         <v>31</v>
       </c>
       <c r="E14" s="9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>9</v>
       </c>
-      <c r="F14" s="75">
-        <v>1</v>
-      </c>
-      <c r="G14" s="75" t="s">
+      <c r="F14" s="74">
+        <v>1</v>
+      </c>
+      <c r="G14" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="H14" s="96">
-        <v>0</v>
-      </c>
-      <c r="I14" s="76" t="s">
+      <c r="H14" s="95">
+        <v>0</v>
+      </c>
+      <c r="I14" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="J14" s="96">
-        <v>0</v>
-      </c>
-      <c r="K14" s="43">
+      <c r="J14" s="95">
+        <v>0</v>
+      </c>
+      <c r="K14" s="42">
         <v>-1</v>
       </c>
-      <c r="L14" s="96">
-        <v>0</v>
-      </c>
-      <c r="M14" s="43">
+      <c r="L14" s="95">
+        <v>0</v>
+      </c>
+      <c r="M14" s="42">
         <f>M18</f>
         <v>2000000</v>
       </c>
-      <c r="N14" s="96">
-        <v>0</v>
-      </c>
-      <c r="O14" s="43">
-        <v>1</v>
-      </c>
-      <c r="P14" s="77">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="77">
-        <v>1</v>
-      </c>
-      <c r="R14" s="96">
-        <v>1</v>
-      </c>
-      <c r="S14" s="96">
-        <v>0</v>
-      </c>
-      <c r="T14" s="96">
-        <v>0</v>
-      </c>
-      <c r="U14" s="96">
-        <v>0</v>
-      </c>
-      <c r="V14" s="97">
-        <v>0</v>
-      </c>
-      <c r="W14" s="96">
+      <c r="N14" s="95">
+        <v>0</v>
+      </c>
+      <c r="O14" s="42">
+        <v>1</v>
+      </c>
+      <c r="P14" s="76">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="76">
+        <v>1</v>
+      </c>
+      <c r="R14" s="95">
+        <v>1</v>
+      </c>
+      <c r="S14" s="95">
+        <v>0</v>
+      </c>
+      <c r="T14" s="95">
+        <v>0</v>
+      </c>
+      <c r="U14" s="95">
+        <v>0</v>
+      </c>
+      <c r="V14" s="96">
+        <v>0</v>
+      </c>
+      <c r="W14" s="95">
         <v>2.3E-2</v>
       </c>
-      <c r="X14" s="96">
-        <v>0</v>
-      </c>
-      <c r="Y14" s="43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:25" s="62" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="122"/>
-      <c r="B15" s="59" t="s">
+      <c r="X14" s="95">
+        <v>0</v>
+      </c>
+      <c r="Y14" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" s="61" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="120"/>
+      <c r="B15" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="60" t="s">
-        <v>150</v>
-      </c>
-      <c r="D15" s="99" t="s">
+      <c r="C15" s="59" t="s">
+        <v>149</v>
+      </c>
+      <c r="D15" s="98" t="s">
+        <v>153</v>
+      </c>
+      <c r="E15" s="9">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="F15" s="60">
+        <v>1</v>
+      </c>
+      <c r="G15" s="60" t="s">
+        <v>117</v>
+      </c>
+      <c r="H15" s="61">
+        <v>0</v>
+      </c>
+      <c r="I15" s="115" t="s">
+        <v>12</v>
+      </c>
+      <c r="J15" s="61">
+        <v>0</v>
+      </c>
+      <c r="K15" s="61">
+        <v>0</v>
+      </c>
+      <c r="L15" s="61">
+        <v>-1</v>
+      </c>
+      <c r="M15" s="61">
+        <v>20000</v>
+      </c>
+      <c r="N15" s="63">
+        <v>0</v>
+      </c>
+      <c r="O15" s="61">
+        <v>0</v>
+      </c>
+      <c r="P15" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="62">
+        <v>1</v>
+      </c>
+      <c r="R15" s="61">
+        <v>1</v>
+      </c>
+      <c r="S15" s="61">
+        <v>0.94</v>
+      </c>
+      <c r="T15" s="61">
+        <v>0</v>
+      </c>
+      <c r="U15" s="61">
+        <v>0</v>
+      </c>
+      <c r="V15" s="61">
+        <v>0</v>
+      </c>
+      <c r="W15" s="61">
+        <v>0</v>
+      </c>
+      <c r="X15" s="61">
+        <v>0</v>
+      </c>
+      <c r="Y15" s="61">
+        <v>9.3678779051968114E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" s="61" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="120"/>
+      <c r="B16" s="58" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="59" t="s">
+        <v>149</v>
+      </c>
+      <c r="D16" s="98" t="s">
         <v>154</v>
       </c>
-      <c r="E15" s="9">
-        <f t="shared" si="6"/>
-        <v>10</v>
-      </c>
-      <c r="F15" s="61">
-        <v>1</v>
-      </c>
-      <c r="G15" s="61" t="s">
-        <v>117</v>
-      </c>
-      <c r="H15" s="62">
-        <v>0</v>
-      </c>
-      <c r="I15" s="117" t="s">
+      <c r="E16" s="9">
+        <f t="shared" si="7"/>
+        <v>11</v>
+      </c>
+      <c r="F16" s="60">
+        <v>1</v>
+      </c>
+      <c r="G16" s="60" t="s">
+        <v>118</v>
+      </c>
+      <c r="H16" s="61">
+        <v>0</v>
+      </c>
+      <c r="I16" s="115" t="s">
         <v>12</v>
       </c>
-      <c r="J15" s="62">
-        <v>0</v>
-      </c>
-      <c r="K15" s="62">
-        <v>0</v>
-      </c>
-      <c r="L15" s="62">
-        <v>-1</v>
-      </c>
-      <c r="M15" s="62">
+      <c r="J16" s="61">
+        <v>0</v>
+      </c>
+      <c r="K16" s="61">
+        <v>0</v>
+      </c>
+      <c r="L16" s="61">
+        <v>1</v>
+      </c>
+      <c r="M16" s="61">
         <v>20000</v>
       </c>
-      <c r="N15" s="64">
-        <v>0</v>
-      </c>
-      <c r="O15" s="62">
-        <v>0</v>
-      </c>
-      <c r="P15" s="63">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="63">
-        <v>1</v>
-      </c>
-      <c r="R15" s="62">
-        <v>1</v>
-      </c>
-      <c r="S15" s="62">
-        <v>0.94</v>
-      </c>
-      <c r="T15" s="62">
-        <v>0</v>
-      </c>
-      <c r="U15" s="62">
-        <v>0</v>
-      </c>
-      <c r="V15" s="62">
-        <v>0</v>
-      </c>
-      <c r="W15" s="62">
-        <v>0</v>
-      </c>
-      <c r="X15" s="62">
-        <v>0</v>
-      </c>
-      <c r="Y15" s="62">
-        <v>9.3678779051968114E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:25" s="62" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="122"/>
-      <c r="B16" s="59" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="60" t="s">
-        <v>150</v>
-      </c>
-      <c r="D16" s="99" t="s">
+      <c r="N16" s="63">
+        <v>0</v>
+      </c>
+      <c r="O16" s="61">
+        <v>0</v>
+      </c>
+      <c r="P16" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="62">
+        <v>1</v>
+      </c>
+      <c r="R16" s="61">
+        <v>1</v>
+      </c>
+      <c r="S16" s="61">
+        <v>0</v>
+      </c>
+      <c r="T16" s="61">
+        <v>0</v>
+      </c>
+      <c r="U16" s="61">
+        <v>0</v>
+      </c>
+      <c r="V16" s="61">
+        <v>0</v>
+      </c>
+      <c r="W16" s="61">
+        <v>0</v>
+      </c>
+      <c r="X16" s="61">
+        <v>0</v>
+      </c>
+      <c r="Y16" s="61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" s="103" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="120"/>
+      <c r="B17" s="99" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="100" t="s">
+        <v>149</v>
+      </c>
+      <c r="D17" s="101" t="s">
         <v>155</v>
       </c>
-      <c r="E16" s="9">
-        <f t="shared" si="6"/>
-        <v>11</v>
-      </c>
-      <c r="F16" s="61">
-        <v>1</v>
-      </c>
-      <c r="G16" s="61" t="s">
-        <v>118</v>
-      </c>
-      <c r="H16" s="62">
-        <v>0</v>
-      </c>
-      <c r="I16" s="117" t="s">
+      <c r="E17" s="97">
+        <f t="shared" si="7"/>
         <v>12</v>
       </c>
-      <c r="J16" s="62">
-        <v>0</v>
-      </c>
-      <c r="K16" s="62">
-        <v>0</v>
-      </c>
-      <c r="L16" s="62">
-        <v>1</v>
-      </c>
-      <c r="M16" s="62">
-        <v>20000</v>
-      </c>
-      <c r="N16" s="64">
-        <v>0</v>
-      </c>
-      <c r="O16" s="62">
-        <v>0</v>
-      </c>
-      <c r="P16" s="63">
-        <v>0</v>
-      </c>
-      <c r="Q16" s="63">
-        <v>1</v>
-      </c>
-      <c r="R16" s="62">
-        <v>1</v>
-      </c>
-      <c r="S16" s="62">
-        <v>0</v>
-      </c>
-      <c r="T16" s="62">
-        <v>0</v>
-      </c>
-      <c r="U16" s="62">
-        <v>0</v>
-      </c>
-      <c r="V16" s="62">
-        <v>0</v>
-      </c>
-      <c r="W16" s="62">
-        <v>0</v>
-      </c>
-      <c r="X16" s="62">
-        <v>0</v>
-      </c>
-      <c r="Y16" s="62">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:25" s="104" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="122"/>
-      <c r="B17" s="100" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="101" t="s">
-        <v>150</v>
-      </c>
-      <c r="D17" s="102" t="s">
-        <v>156</v>
-      </c>
-      <c r="E17" s="98">
-        <f t="shared" si="6"/>
+      <c r="F17" s="102">
+        <v>1</v>
+      </c>
+      <c r="G17" s="102" t="s">
+        <v>119</v>
+      </c>
+      <c r="H17" s="103">
+        <v>0</v>
+      </c>
+      <c r="I17" s="116" t="s">
         <v>12</v>
       </c>
-      <c r="F17" s="103">
-        <v>1</v>
-      </c>
-      <c r="G17" s="103" t="s">
-        <v>119</v>
-      </c>
-      <c r="H17" s="104">
-        <v>0</v>
-      </c>
-      <c r="I17" s="118" t="s">
-        <v>12</v>
-      </c>
-      <c r="J17" s="104">
-        <v>0</v>
-      </c>
-      <c r="K17" s="104">
-        <v>0</v>
-      </c>
-      <c r="L17" s="104">
-        <v>0</v>
-      </c>
-      <c r="M17" s="104">
+      <c r="J17" s="103">
+        <v>0</v>
+      </c>
+      <c r="K17" s="103">
+        <v>0</v>
+      </c>
+      <c r="L17" s="103">
+        <v>0</v>
+      </c>
+      <c r="M17" s="103">
         <v>20000000</v>
       </c>
-      <c r="N17" s="104">
-        <v>0</v>
-      </c>
-      <c r="O17" s="104">
-        <v>0</v>
-      </c>
-      <c r="P17" s="105">
+      <c r="N17" s="103">
+        <v>0</v>
+      </c>
+      <c r="O17" s="103">
+        <v>0</v>
+      </c>
+      <c r="P17" s="104">
         <v>0.09</v>
       </c>
-      <c r="Q17" s="105">
-        <v>1</v>
-      </c>
-      <c r="R17" s="104">
-        <v>1</v>
-      </c>
-      <c r="S17" s="104">
-        <v>0</v>
-      </c>
-      <c r="T17" s="104">
+      <c r="Q17" s="104">
+        <v>1</v>
+      </c>
+      <c r="R17" s="103">
+        <v>1</v>
+      </c>
+      <c r="S17" s="103">
+        <v>0</v>
+      </c>
+      <c r="T17" s="103">
         <v>460.75542459148141</v>
       </c>
-      <c r="U17" s="104">
+      <c r="U17" s="103">
         <v>0.99167600700525393</v>
       </c>
-      <c r="V17" s="104">
-        <v>0</v>
-      </c>
-      <c r="W17" s="104">
-        <v>0</v>
-      </c>
-      <c r="X17" s="104">
-        <v>0</v>
-      </c>
-      <c r="Y17" s="104">
+      <c r="V17" s="103">
+        <v>0</v>
+      </c>
+      <c r="W17" s="103">
+        <v>0</v>
+      </c>
+      <c r="X17" s="103">
+        <v>0</v>
+      </c>
+      <c r="Y17" s="103">
         <v>8.174285816161557E-2</v>
       </c>
     </row>
     <row r="18" spans="1:25" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="125" t="s">
+      <c r="A18" s="123" t="s">
         <v>17</v>
       </c>
       <c r="B18" s="12" t="s">
         <v>42</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D18" s="7" t="s">
         <v>37</v>
       </c>
       <c r="E18" s="9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>13</v>
       </c>
       <c r="F18" s="2">
@@ -3278,7 +3293,7 @@
       <c r="H18">
         <v>0</v>
       </c>
-      <c r="I18" s="115" t="s">
+      <c r="I18" s="113" t="s">
         <v>12</v>
       </c>
       <c r="J18">
@@ -3331,12 +3346,12 @@
       </c>
     </row>
     <row r="19" spans="1:25" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="125"/>
+      <c r="A19" s="123"/>
       <c r="B19" s="12" t="s">
         <v>41</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>39</v>
@@ -3354,7 +3369,7 @@
       <c r="H19">
         <v>0</v>
       </c>
-      <c r="I19" s="115" t="s">
+      <c r="I19" s="113" t="s">
         <v>12</v>
       </c>
       <c r="J19">
@@ -3367,7 +3382,7 @@
         <v>0</v>
       </c>
       <c r="M19">
-        <f t="shared" ref="M19:M32" si="7">$M$18</f>
+        <f t="shared" ref="M19:M32" si="8">$M$18</f>
         <v>2000000</v>
       </c>
       <c r="N19" s="10">
@@ -3408,19 +3423,19 @@
       </c>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A20" s="125"/>
+      <c r="A20" s="123"/>
       <c r="B20" s="12" t="str">
         <f>CONCATENATE("RPU_"&amp;D20)</f>
         <v>RPU_ON_SP198-HH100</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>120</v>
       </c>
       <c r="E20" s="9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>15</v>
       </c>
       <c r="F20" s="2">
@@ -3432,7 +3447,7 @@
       <c r="H20">
         <v>0</v>
       </c>
-      <c r="I20" s="115" t="s">
+      <c r="I20" s="113" t="s">
         <v>12</v>
       </c>
       <c r="J20">
@@ -3445,7 +3460,7 @@
         <v>0</v>
       </c>
       <c r="M20">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2000000</v>
       </c>
       <c r="N20" s="10">
@@ -3486,19 +3501,19 @@
       </c>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A21" s="125"/>
+      <c r="A21" s="123"/>
       <c r="B21" s="12" t="str">
-        <f t="shared" ref="B21:B31" si="8">CONCATENATE("RPU_"&amp;D21)</f>
+        <f t="shared" ref="B21:B31" si="9">CONCATENATE("RPU_"&amp;D21)</f>
         <v>RPU_ON_SP198-HH150</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>44</v>
       </c>
       <c r="E21" s="9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
       <c r="F21" s="2">
@@ -3510,7 +3525,7 @@
       <c r="H21">
         <v>0</v>
       </c>
-      <c r="I21" s="115" t="s">
+      <c r="I21" s="113" t="s">
         <v>12</v>
       </c>
       <c r="J21">
@@ -3523,7 +3538,7 @@
         <v>0</v>
       </c>
       <c r="M21">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2000000</v>
       </c>
       <c r="N21" s="10">
@@ -3564,19 +3579,19 @@
       </c>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A22" s="125"/>
+      <c r="A22" s="123"/>
       <c r="B22" s="12" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>RPU_ON_SP237-HH100</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>46</v>
       </c>
       <c r="E22" s="9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>17</v>
       </c>
       <c r="F22" s="2">
@@ -3588,7 +3603,7 @@
       <c r="H22">
         <v>0</v>
       </c>
-      <c r="I22" s="115" t="s">
+      <c r="I22" s="113" t="s">
         <v>12</v>
       </c>
       <c r="J22">
@@ -3601,7 +3616,7 @@
         <v>0</v>
       </c>
       <c r="M22">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2000000</v>
       </c>
       <c r="N22" s="10">
@@ -3642,19 +3657,19 @@
       </c>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A23" s="125"/>
+      <c r="A23" s="123"/>
       <c r="B23" s="12" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>RPU_ON_SP237-HH150</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>48</v>
       </c>
       <c r="E23" s="9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>18</v>
       </c>
       <c r="F23" s="2">
@@ -3666,7 +3681,7 @@
       <c r="H23">
         <v>0</v>
       </c>
-      <c r="I23" s="115" t="s">
+      <c r="I23" s="113" t="s">
         <v>12</v>
       </c>
       <c r="J23">
@@ -3679,7 +3694,7 @@
         <v>0</v>
       </c>
       <c r="M23">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2000000</v>
       </c>
       <c r="N23" s="10">
@@ -3720,19 +3735,19 @@
       </c>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A24" s="125"/>
+      <c r="A24" s="123"/>
       <c r="B24" s="12" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>RPU_ON_SP277-HH100</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>50</v>
       </c>
       <c r="E24" s="9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>19</v>
       </c>
       <c r="F24" s="2">
@@ -3744,7 +3759,7 @@
       <c r="H24">
         <v>0</v>
       </c>
-      <c r="I24" s="115" t="s">
+      <c r="I24" s="113" t="s">
         <v>12</v>
       </c>
       <c r="J24">
@@ -3757,7 +3772,7 @@
         <v>0</v>
       </c>
       <c r="M24">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2000000</v>
       </c>
       <c r="N24" s="10">
@@ -3798,19 +3813,19 @@
       </c>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A25" s="125"/>
+      <c r="A25" s="123"/>
       <c r="B25" s="12" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>RPU_ON_SP277-HH150</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>52</v>
       </c>
       <c r="E25" s="9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>20</v>
       </c>
       <c r="F25" s="2">
@@ -3822,7 +3837,7 @@
       <c r="H25">
         <v>0</v>
       </c>
-      <c r="I25" s="115" t="s">
+      <c r="I25" s="113" t="s">
         <v>12</v>
       </c>
       <c r="J25">
@@ -3835,7 +3850,7 @@
         <v>0</v>
       </c>
       <c r="M25">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2000000</v>
       </c>
       <c r="N25" s="10">
@@ -3876,19 +3891,19 @@
       </c>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A26" s="125"/>
+      <c r="A26" s="123"/>
       <c r="B26" s="12" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>RPU_ON_SP321-HH100</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>54</v>
       </c>
       <c r="E26" s="9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>21</v>
       </c>
       <c r="F26" s="2">
@@ -3900,7 +3915,7 @@
       <c r="H26">
         <v>0</v>
       </c>
-      <c r="I26" s="115" t="s">
+      <c r="I26" s="113" t="s">
         <v>12</v>
       </c>
       <c r="J26">
@@ -3913,7 +3928,7 @@
         <v>0</v>
       </c>
       <c r="M26">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2000000</v>
       </c>
       <c r="N26" s="10">
@@ -3954,19 +3969,19 @@
       </c>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A27" s="125"/>
+      <c r="A27" s="123"/>
       <c r="B27" s="12" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>RPU_ON_SP321-HH150</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>56</v>
       </c>
       <c r="E27" s="9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>22</v>
       </c>
       <c r="F27" s="2">
@@ -3978,7 +3993,7 @@
       <c r="H27">
         <v>0</v>
       </c>
-      <c r="I27" s="115" t="s">
+      <c r="I27" s="113" t="s">
         <v>12</v>
       </c>
       <c r="J27">
@@ -3991,7 +4006,7 @@
         <v>0</v>
       </c>
       <c r="M27">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2000000</v>
       </c>
       <c r="N27" s="10">
@@ -4032,19 +4047,19 @@
       </c>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A28" s="125"/>
+      <c r="A28" s="123"/>
       <c r="B28" s="12" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>RPU_OFF_SP379-HH100</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>58</v>
       </c>
       <c r="E28" s="9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>23</v>
       </c>
       <c r="F28" s="2">
@@ -4056,7 +4071,7 @@
       <c r="H28">
         <v>0</v>
       </c>
-      <c r="I28" s="115" t="s">
+      <c r="I28" s="113" t="s">
         <v>12</v>
       </c>
       <c r="J28">
@@ -4069,7 +4084,7 @@
         <v>0</v>
       </c>
       <c r="M28">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2000000</v>
       </c>
       <c r="N28" s="10">
@@ -4110,19 +4125,19 @@
       </c>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A29" s="125"/>
+      <c r="A29" s="123"/>
       <c r="B29" s="12" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>RPU_OFF_SP379-HH150</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>60</v>
       </c>
       <c r="E29" s="9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>24</v>
       </c>
       <c r="F29" s="2">
@@ -4134,7 +4149,7 @@
       <c r="H29">
         <v>0</v>
       </c>
-      <c r="I29" s="115" t="s">
+      <c r="I29" s="113" t="s">
         <v>12</v>
       </c>
       <c r="J29">
@@ -4147,7 +4162,7 @@
         <v>0</v>
       </c>
       <c r="M29">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2000000</v>
       </c>
       <c r="N29" s="10">
@@ -4188,19 +4203,19 @@
       </c>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A30" s="125"/>
+      <c r="A30" s="123"/>
       <c r="B30" s="12" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>RPU_OFF_SP450-HH100</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>62</v>
       </c>
       <c r="E30" s="9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>25</v>
       </c>
       <c r="F30" s="2">
@@ -4212,7 +4227,7 @@
       <c r="H30">
         <v>0</v>
       </c>
-      <c r="I30" s="115" t="s">
+      <c r="I30" s="113" t="s">
         <v>12</v>
       </c>
       <c r="J30">
@@ -4225,7 +4240,7 @@
         <v>0</v>
       </c>
       <c r="M30">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2000000</v>
       </c>
       <c r="N30" s="10">
@@ -4266,19 +4281,19 @@
       </c>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A31" s="125"/>
+      <c r="A31" s="123"/>
       <c r="B31" s="12" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>RPU_OFF_SP450-HH150</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>121</v>
       </c>
       <c r="E31" s="9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>26</v>
       </c>
       <c r="F31" s="2">
@@ -4290,7 +4305,7 @@
       <c r="H31">
         <v>0</v>
       </c>
-      <c r="I31" s="115" t="s">
+      <c r="I31" s="113" t="s">
         <v>12</v>
       </c>
       <c r="J31">
@@ -4303,7 +4318,7 @@
         <v>0</v>
       </c>
       <c r="M31">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2000000</v>
       </c>
       <c r="N31" s="10">
@@ -4344,7 +4359,7 @@
       </c>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A32" s="125"/>
+      <c r="A32" s="123"/>
       <c r="B32" s="12" t="s">
         <v>25</v>
       </c>
@@ -4355,7 +4370,7 @@
         <v>33</v>
       </c>
       <c r="E32" s="9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>27</v>
       </c>
       <c r="F32" s="2">
@@ -4367,7 +4382,7 @@
       <c r="H32">
         <v>0</v>
       </c>
-      <c r="I32" s="115" t="s">
+      <c r="I32" s="113" t="s">
         <v>12</v>
       </c>
       <c r="J32">
@@ -4380,7 +4395,7 @@
         <v>0</v>
       </c>
       <c r="M32">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2000000</v>
       </c>
       <c r="N32" s="10">
@@ -4413,7 +4428,7 @@
       <c r="W32">
         <v>0</v>
       </c>
-      <c r="X32" s="28">
+      <c r="X32" s="27">
         <v>1.6649999999999998E-2</v>
       </c>
       <c r="Y32">
@@ -4421,30 +4436,30 @@
       </c>
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A33" s="125"/>
+      <c r="A33" s="123"/>
       <c r="B33" s="12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C33" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="D33" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="D33" s="7" t="s">
-        <v>151</v>
-      </c>
       <c r="E33" s="9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>28</v>
       </c>
       <c r="F33" s="2">
         <v>1</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H33">
         <v>0</v>
       </c>
-      <c r="I33" s="115" t="s">
+      <c r="I33" s="113" t="s">
         <v>12</v>
       </c>
       <c r="J33">
@@ -4497,18 +4512,18 @@
       </c>
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A34" s="125"/>
+      <c r="A34" s="123"/>
       <c r="B34" s="12" t="s">
         <v>14</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D34" s="7" t="s">
         <v>34</v>
       </c>
       <c r="E34" s="9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>29</v>
       </c>
       <c r="F34" s="2">
@@ -4520,7 +4535,7 @@
       <c r="H34">
         <v>0</v>
       </c>
-      <c r="I34" s="115" t="s">
+      <c r="I34" s="113" t="s">
         <v>12</v>
       </c>
       <c r="J34">
@@ -4574,18 +4589,18 @@
       </c>
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A35" s="125"/>
+      <c r="A35" s="123"/>
       <c r="B35" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D35" s="7" t="s">
         <v>35</v>
       </c>
       <c r="E35" s="9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>30</v>
       </c>
       <c r="F35" s="2">
@@ -4597,7 +4612,7 @@
       <c r="H35">
         <v>0</v>
       </c>
-      <c r="I35" s="115" t="s">
+      <c r="I35" s="113" t="s">
         <v>12</v>
       </c>
       <c r="J35">
@@ -4651,18 +4666,18 @@
       </c>
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A36" s="125"/>
+      <c r="A36" s="123"/>
       <c r="B36" s="12" t="s">
         <v>16</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>36</v>
       </c>
       <c r="E36" s="9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>31</v>
       </c>
       <c r="F36" s="2">
@@ -4674,7 +4689,7 @@
       <c r="H36">
         <v>0</v>
       </c>
-      <c r="I36" s="115" t="s">
+      <c r="I36" s="113" t="s">
         <v>12</v>
       </c>
       <c r="J36">
@@ -4744,7 +4759,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="I17" sqref="I17"/>
     </sheetView>
@@ -4758,7 +4773,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="57"/>
+      <c r="A1" s="56"/>
       <c r="B1" s="6" t="s">
         <v>122</v>
       </c>
@@ -4770,19 +4785,19 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="58"/>
+      <c r="A2" s="57"/>
       <c r="B2" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="C2" s="29">
+      <c r="C2" s="28">
         <v>18.600000000000001</v>
       </c>
-      <c r="D2" s="29">
+      <c r="D2" s="28">
         <v>18.600000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="57"/>
+      <c r="A3" s="56"/>
       <c r="B3" t="s">
         <v>84</v>
       </c>
@@ -4794,7 +4809,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="58"/>
+      <c r="A4" s="57"/>
       <c r="B4" t="s">
         <v>95</v>
       </c>
@@ -4864,10 +4879,10 @@
         <f>Data_base_case!D8</f>
         <v>Water supply (desalination plant)</v>
       </c>
-      <c r="C8" s="49">
-        <v>1</v>
-      </c>
-      <c r="D8" s="49">
+      <c r="C8" s="48">
+        <v>1</v>
+      </c>
+      <c r="D8" s="48">
         <v>1</v>
       </c>
     </row>
@@ -5018,10 +5033,10 @@
         <f>Data_base_case!D17</f>
         <v>H2 storage (buried pipes)</v>
       </c>
-      <c r="C17" s="49">
-        <v>1</v>
-      </c>
-      <c r="D17" s="49">
+      <c r="C17" s="48">
+        <v>1</v>
+      </c>
+      <c r="D17" s="48">
         <v>1</v>
       </c>
     </row>
@@ -5034,10 +5049,10 @@
         <f>Data_base_case!D18</f>
         <v>Solar fixed</v>
       </c>
-      <c r="C18" s="49">
-        <v>1</v>
-      </c>
-      <c r="D18" s="49">
+      <c r="C18" s="48">
+        <v>1</v>
+      </c>
+      <c r="D18" s="48">
         <v>1</v>
       </c>
     </row>
@@ -5050,10 +5065,10 @@
         <f>Data_base_case!D19</f>
         <v>Solar tracking</v>
       </c>
-      <c r="C19" s="49">
-        <v>1</v>
-      </c>
-      <c r="D19" s="49">
+      <c r="C19" s="48">
+        <v>1</v>
+      </c>
+      <c r="D19" s="48">
         <v>1</v>
       </c>
     </row>
@@ -5066,10 +5081,10 @@
         <f>Data_base_case!D20</f>
         <v>ON_SP198-HH100</v>
       </c>
-      <c r="C20" s="49">
-        <v>1</v>
-      </c>
-      <c r="D20" s="49">
+      <c r="C20" s="48">
+        <v>1</v>
+      </c>
+      <c r="D20" s="48">
         <v>1</v>
       </c>
     </row>
@@ -5082,10 +5097,10 @@
         <f>Data_base_case!D21</f>
         <v>ON_SP198-HH150</v>
       </c>
-      <c r="C21" s="49">
-        <v>1</v>
-      </c>
-      <c r="D21" s="49">
+      <c r="C21" s="48">
+        <v>1</v>
+      </c>
+      <c r="D21" s="48">
         <v>1</v>
       </c>
     </row>
@@ -5098,10 +5113,10 @@
         <f>Data_base_case!D22</f>
         <v>ON_SP237-HH100</v>
       </c>
-      <c r="C22" s="49">
-        <v>1</v>
-      </c>
-      <c r="D22" s="49">
+      <c r="C22" s="48">
+        <v>1</v>
+      </c>
+      <c r="D22" s="48">
         <v>1</v>
       </c>
     </row>
@@ -5114,10 +5129,10 @@
         <f>Data_base_case!D23</f>
         <v>ON_SP237-HH150</v>
       </c>
-      <c r="C23" s="49">
-        <v>1</v>
-      </c>
-      <c r="D23" s="49">
+      <c r="C23" s="48">
+        <v>1</v>
+      </c>
+      <c r="D23" s="48">
         <v>1</v>
       </c>
     </row>
@@ -5130,10 +5145,10 @@
         <f>Data_base_case!D24</f>
         <v>ON_SP277-HH100</v>
       </c>
-      <c r="C24" s="49">
-        <v>1</v>
-      </c>
-      <c r="D24" s="49">
+      <c r="C24" s="48">
+        <v>1</v>
+      </c>
+      <c r="D24" s="48">
         <v>1</v>
       </c>
     </row>
@@ -5146,10 +5161,10 @@
         <f>Data_base_case!D25</f>
         <v>ON_SP277-HH150</v>
       </c>
-      <c r="C25" s="49">
-        <v>1</v>
-      </c>
-      <c r="D25" s="49">
+      <c r="C25" s="48">
+        <v>1</v>
+      </c>
+      <c r="D25" s="48">
         <v>1</v>
       </c>
     </row>
@@ -5162,10 +5177,10 @@
         <f>Data_base_case!D26</f>
         <v>ON_SP321-HH100</v>
       </c>
-      <c r="C26" s="49">
-        <v>1</v>
-      </c>
-      <c r="D26" s="49">
+      <c r="C26" s="48">
+        <v>1</v>
+      </c>
+      <c r="D26" s="48">
         <v>1</v>
       </c>
     </row>
@@ -5178,10 +5193,10 @@
         <f>Data_base_case!D27</f>
         <v>ON_SP321-HH150</v>
       </c>
-      <c r="C27" s="49">
-        <v>1</v>
-      </c>
-      <c r="D27" s="49">
+      <c r="C27" s="48">
+        <v>1</v>
+      </c>
+      <c r="D27" s="48">
         <v>1</v>
       </c>
     </row>
@@ -5374,17 +5389,17 @@
   <sheetData>
     <row r="1" spans="1:140" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:140" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4" spans="1:140" s="16" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="33" t="s">
-        <v>134</v>
+      <c r="A4" s="32" t="s">
+        <v>133</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>105</v>
@@ -5677,7 +5692,7 @@
       </c>
       <c r="CC4" s="16" t="str">
         <f>Data_base_case!V2&amp;Data_base_case!V3</f>
-        <v>Variable cost (EUR/Output)2020</v>
+        <v>Variable cost (EUR/output)2020</v>
       </c>
       <c r="CD4" s="16" t="e">
         <f>Data_base_case!#REF!&amp;Data_base_case!#REF!</f>
@@ -5917,9 +5932,9 @@
       </c>
     </row>
     <row r="5" spans="1:140" s="16" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="36"/>
+      <c r="A5" s="35"/>
       <c r="B5" s="16" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C5" s="16" t="s">
         <v>33</v>
@@ -5934,7 +5949,7 @@
       <c r="F5" s="16">
         <v>1</v>
       </c>
-      <c r="G5" s="37" t="s">
+      <c r="G5" s="36" t="s">
         <v>100</v>
       </c>
       <c r="H5" s="16">
@@ -5943,36 +5958,36 @@
       </c>
     </row>
     <row r="6" spans="1:140" s="16" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="36" t="str">
+      <c r="A6" s="35" t="str">
         <f>B5</f>
         <v>Semi-islanded</v>
       </c>
-      <c r="B6" s="39" t="s">
-        <v>138</v>
-      </c>
-      <c r="C6" s="39" t="s">
-        <v>157</v>
-      </c>
-      <c r="D6" s="39" t="str">
+      <c r="B6" s="38" t="s">
+        <v>137</v>
+      </c>
+      <c r="C6" s="38" t="s">
+        <v>156</v>
+      </c>
+      <c r="D6" s="38" t="str">
         <f>Data_base_case!$P$1</f>
         <v>Load min (% of max capacity)</v>
       </c>
-      <c r="E6" s="39" t="s">
+      <c r="E6" s="38" t="s">
         <v>100</v>
       </c>
-      <c r="F6" s="39">
-        <v>0</v>
-      </c>
-      <c r="G6" s="40">
+      <c r="F6" s="38">
+        <v>0</v>
+      </c>
+      <c r="G6" s="39">
         <v>2020</v>
       </c>
-      <c r="H6" s="39">
+      <c r="H6" s="38">
         <f>INDEX(Data_base_case!$D$5:$Y$82,MATCH(Scenarios_definition!C6,Data_base_case!$D$5:$D$82,0),MATCH(Scenarios_definition!D6&amp;Scenarios_definition!G6,Data_base_case!$D$4:$Y$4,0))</f>
         <v>0.4</v>
       </c>
     </row>
     <row r="7" spans="1:140" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="22"/>
+      <c r="A7" s="21"/>
       <c r="B7" s="1" t="s">
         <v>111</v>
       </c>
@@ -5990,7 +6005,7 @@
       <c r="F7" s="1">
         <v>0</v>
       </c>
-      <c r="G7" s="21" t="s">
+      <c r="G7" s="20" t="s">
         <v>100</v>
       </c>
       <c r="H7" s="1">
@@ -5998,27 +6013,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:140" s="31" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="22" t="s">
+    <row r="8" spans="1:140" s="30" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="21" t="s">
         <v>111</v>
       </c>
-      <c r="B8" s="31" t="s">
+      <c r="B8" s="30" t="s">
         <v>124</v>
       </c>
-      <c r="C8" s="31" t="s">
-        <v>157</v>
-      </c>
-      <c r="D8" s="31" t="str">
+      <c r="C8" s="30" t="s">
+        <v>156</v>
+      </c>
+      <c r="D8" s="30" t="str">
         <f>Data_base_case!$P$1</f>
         <v>Load min (% of max capacity)</v>
       </c>
-      <c r="E8" s="31" t="s">
+      <c r="E8" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="F8" s="31">
-        <v>1</v>
-      </c>
-      <c r="G8" s="32">
+      <c r="F8" s="30">
+        <v>1</v>
+      </c>
+      <c r="G8" s="31">
         <v>2020</v>
       </c>
       <c r="H8" s="1">
@@ -6026,25 +6041,25 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="9" spans="1:140" s="24" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="23"/>
-      <c r="B9" s="24" t="s">
+    <row r="9" spans="1:140" s="23" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="22"/>
+      <c r="B9" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="C9" s="24" t="s">
-        <v>157</v>
-      </c>
-      <c r="D9" s="24" t="str">
+      <c r="C9" s="23" t="s">
+        <v>156</v>
+      </c>
+      <c r="D9" s="23" t="str">
         <f>Data_base_case!$P$1</f>
         <v>Load min (% of max capacity)</v>
       </c>
-      <c r="E9" s="24" t="s">
+      <c r="E9" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="F9" s="24">
-        <v>1</v>
-      </c>
-      <c r="G9" s="25">
+      <c r="F9" s="23">
+        <v>1</v>
+      </c>
+      <c r="G9" s="24">
         <v>2020</v>
       </c>
       <c r="H9" s="1">
@@ -6052,30 +6067,30 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="10" spans="1:140" s="41" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:140" s="40" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B10" s="41" t="s">
-        <v>139</v>
-      </c>
-      <c r="C10" s="41" t="s">
-        <v>157</v>
-      </c>
-      <c r="D10" s="41" t="str">
+      <c r="B10" s="40" t="s">
+        <v>138</v>
+      </c>
+      <c r="C10" s="40" t="s">
+        <v>156</v>
+      </c>
+      <c r="D10" s="40" t="str">
         <f>Data_base_case!$P$1</f>
         <v>Load min (% of max capacity)</v>
       </c>
-      <c r="E10" s="41" t="s">
+      <c r="E10" s="40" t="s">
         <v>100</v>
       </c>
-      <c r="F10" s="41">
-        <v>0</v>
-      </c>
-      <c r="G10" s="42">
+      <c r="F10" s="40">
+        <v>0</v>
+      </c>
+      <c r="G10" s="41">
         <v>2020</v>
       </c>
-      <c r="H10" s="41">
+      <c r="H10" s="40">
         <f>INDEX(Data_base_case!$D$5:$Y$82,MATCH(Scenarios_definition!C10,Data_base_case!$D$5:$D$82,0),MATCH(Scenarios_definition!D10&amp;Scenarios_definition!G10,Data_base_case!$D$4:$Y$4,0))</f>
         <v>0.4</v>
       </c>
@@ -6118,29 +6133,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="B1" s="128" t="s">
+      <c r="B1" s="126" t="s">
         <v>108</v>
       </c>
-      <c r="C1" s="128"/>
-      <c r="D1" s="128"/>
-      <c r="E1" s="128"/>
-      <c r="F1" s="128"/>
-      <c r="G1" s="128"/>
-      <c r="H1" s="128"/>
-      <c r="I1" s="128"/>
-      <c r="J1" s="128"/>
-      <c r="K1" s="128"/>
-      <c r="L1" s="129"/>
+      <c r="C1" s="126"/>
+      <c r="D1" s="126"/>
+      <c r="E1" s="126"/>
+      <c r="F1" s="126"/>
+      <c r="G1" s="126"/>
+      <c r="H1" s="126"/>
+      <c r="I1" s="126"/>
+      <c r="J1" s="126"/>
+      <c r="K1" s="126"/>
+      <c r="L1" s="127"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="130" t="s">
+      <c r="B2" s="128" t="s">
         <v>116</v>
       </c>
-      <c r="C2" s="131" t="s">
+      <c r="C2" s="129" t="s">
         <v>107</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>92</v>
@@ -6151,55 +6166,55 @@
       <c r="G2" s="2">
         <v>2020</v>
       </c>
-      <c r="H2" s="130" t="s">
+      <c r="H2" s="128" t="s">
         <v>128</v>
       </c>
-      <c r="I2" s="130" t="s">
+      <c r="I2" s="128" t="s">
         <v>127</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>73</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="L2" s="54" t="s">
+        <v>135</v>
+      </c>
+      <c r="L2" s="53" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="B3" s="130"/>
-      <c r="C3" s="131"/>
+      <c r="B3" s="128"/>
+      <c r="C3" s="129"/>
       <c r="D3" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
-      <c r="H3" s="130"/>
-      <c r="I3" s="130"/>
+      <c r="H3" s="128"/>
+      <c r="I3" s="128"/>
       <c r="J3" s="2" t="s">
         <v>81</v>
       </c>
       <c r="K3" s="2"/>
-      <c r="L3" s="54"/>
+      <c r="L3" s="53"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="B4" s="130"/>
-      <c r="C4" s="131"/>
+      <c r="B4" s="128"/>
+      <c r="C4" s="129"/>
       <c r="D4" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E4" s="2"/>
       <c r="G4" s="2"/>
-      <c r="H4" s="130"/>
-      <c r="I4" s="130"/>
+      <c r="H4" s="128"/>
+      <c r="I4" s="128"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
-      <c r="L4" s="54"/>
+      <c r="L4" s="53"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="B5" s="130"/>
-      <c r="C5" s="131"/>
+      <c r="B5" s="128"/>
+      <c r="C5" s="129"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -6207,78 +6222,78 @@
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="3"/>
-      <c r="L5" s="30"/>
-      <c r="M5" s="53"/>
+      <c r="L5" s="29"/>
+      <c r="M5" s="52"/>
       <c r="N5" s="3"/>
       <c r="O5" s="3"/>
       <c r="P5" s="3"/>
-      <c r="Q5" s="30"/>
-      <c r="R5" s="55" t="s">
+      <c r="Q5" s="29"/>
+      <c r="R5" s="54" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="K6" s="14"/>
-      <c r="L6" s="38"/>
+      <c r="L6" s="37"/>
       <c r="M6" s="3"/>
       <c r="N6" s="3"/>
       <c r="O6" s="3"/>
       <c r="P6" s="3"/>
-      <c r="Q6" s="30"/>
-    </row>
-    <row r="7" spans="1:18" s="26" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="26" t="s">
+      <c r="Q6" s="29"/>
+    </row>
+    <row r="7" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="25" t="s">
         <v>114</v>
       </c>
-      <c r="D7" s="26" t="s">
-        <v>141</v>
-      </c>
-      <c r="E7" s="26" t="s">
+      <c r="D7" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="E7" s="25" t="s">
         <v>83</v>
       </c>
-      <c r="F7" s="26" t="s">
+      <c r="F7" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="G7" s="26" t="s">
+      <c r="G7" s="25" t="s">
         <v>125</v>
       </c>
-      <c r="H7" s="26" t="s">
+      <c r="H7" s="25" t="s">
         <v>126</v>
       </c>
-      <c r="I7" s="26" t="s">
+      <c r="I7" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="J7" s="26" t="s">
+      <c r="J7" s="25" t="s">
         <v>84</v>
       </c>
-      <c r="K7" s="26" t="s">
+      <c r="K7" s="25" t="s">
         <v>85</v>
       </c>
-      <c r="L7" s="27" t="s">
+      <c r="L7" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="M7" s="26" t="s">
+      <c r="M7" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="N7" s="26" t="s">
+      <c r="N7" s="25" t="s">
         <v>89</v>
       </c>
-      <c r="O7" s="26" t="s">
+      <c r="O7" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="P7" s="26" t="s">
+      <c r="P7" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="Q7" s="27" t="s">
+      <c r="Q7" s="26" t="s">
         <v>98</v>
       </c>
-      <c r="R7" s="26" t="s">
+      <c r="R7" s="25" t="s">
         <v>91</v>
       </c>
     </row>
@@ -6288,13 +6303,13 @@
         <v>1</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C8" s="14" t="s">
         <v>111</v>
       </c>
       <c r="D8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E8" s="14" t="s">
         <v>92</v>
@@ -6302,11 +6317,11 @@
       <c r="F8" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="G8" s="119">
+      <c r="G8" s="117">
         <v>2020</v>
       </c>
       <c r="H8" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I8" s="14" t="str">
         <f t="shared" ref="I8:I25" si="0">"2019"</f>
@@ -6316,10 +6331,10 @@
         <v>73</v>
       </c>
       <c r="K8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L8" s="17" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M8" t="b">
         <v>0</v>
@@ -6346,13 +6361,13 @@
         <v>2</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>111</v>
       </c>
       <c r="D9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E9" s="14" t="s">
         <v>92</v>
@@ -6360,11 +6375,11 @@
       <c r="F9" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="G9" s="119">
+      <c r="G9" s="117">
         <v>2020</v>
       </c>
       <c r="H9" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I9" s="14" t="str">
         <f t="shared" si="0"/>
@@ -6374,10 +6389,10 @@
         <v>73</v>
       </c>
       <c r="K9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L9" s="17" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M9" t="b">
         <v>0</v>
@@ -6404,13 +6419,13 @@
         <v>3</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C10" s="14" t="s">
         <v>111</v>
       </c>
       <c r="D10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E10" s="14" t="s">
         <v>92</v>
@@ -6418,11 +6433,11 @@
       <c r="F10" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="G10" s="119">
+      <c r="G10" s="117">
         <v>2020</v>
       </c>
       <c r="H10" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I10" s="14" t="str">
         <f t="shared" si="0"/>
@@ -6432,10 +6447,10 @@
         <v>73</v>
       </c>
       <c r="K10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L10" s="17" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M10" t="b">
         <v>0</v>
@@ -6462,13 +6477,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E11" s="14" t="s">
         <v>92</v>
@@ -6476,11 +6491,11 @@
       <c r="F11" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="G11" s="52">
+      <c r="G11" s="51">
         <v>2020</v>
       </c>
       <c r="H11" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I11" s="14" t="str">
         <f t="shared" si="0"/>
@@ -6490,10 +6505,10 @@
         <v>73</v>
       </c>
       <c r="K11" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L11" s="17" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M11" t="b">
         <v>0</v>
@@ -6520,13 +6535,13 @@
         <v>5</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E12" s="14" t="s">
         <v>92</v>
@@ -6534,11 +6549,11 @@
       <c r="F12" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="G12" s="52">
+      <c r="G12" s="51">
         <v>2020</v>
       </c>
       <c r="H12" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I12" s="14" t="str">
         <f t="shared" si="0"/>
@@ -6548,10 +6563,10 @@
         <v>73</v>
       </c>
       <c r="K12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L12" s="17" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M12" t="b">
         <v>0</v>
@@ -6578,13 +6593,13 @@
         <v>6</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E13" s="14" t="s">
         <v>92</v>
@@ -6592,11 +6607,11 @@
       <c r="F13" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="G13" s="119">
+      <c r="G13" s="117">
         <v>2020</v>
       </c>
       <c r="H13" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I13" s="14" t="str">
         <f t="shared" si="0"/>
@@ -6606,10 +6621,10 @@
         <v>73</v>
       </c>
       <c r="K13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L13" s="17" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M13" t="b">
         <v>0</v>
@@ -6636,13 +6651,13 @@
         <v>7</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E14" s="14" t="s">
         <v>92</v>
@@ -6650,11 +6665,11 @@
       <c r="F14" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="G14" s="119">
+      <c r="G14" s="117">
         <v>2020</v>
       </c>
       <c r="H14" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I14" s="14" t="str">
         <f t="shared" si="0"/>
@@ -6664,10 +6679,10 @@
         <v>81</v>
       </c>
       <c r="K14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L14" s="17" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M14" t="b">
         <v>0</v>
@@ -6694,13 +6709,13 @@
         <v>8</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D15" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E15" s="14" t="s">
         <v>92</v>
@@ -6708,11 +6723,11 @@
       <c r="F15" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="G15" s="119">
+      <c r="G15" s="117">
         <v>2020</v>
       </c>
       <c r="H15" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I15" s="14" t="str">
         <f t="shared" si="0"/>
@@ -6722,10 +6737,10 @@
         <v>81</v>
       </c>
       <c r="K15" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L15" s="17" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M15" t="b">
         <v>0</v>
@@ -6752,13 +6767,13 @@
         <v>9</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E16" s="14" t="s">
         <v>92</v>
@@ -6766,11 +6781,11 @@
       <c r="F16" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="G16" s="119">
+      <c r="G16" s="117">
         <v>2020</v>
       </c>
       <c r="H16" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I16" s="14" t="str">
         <f t="shared" si="0"/>
@@ -6780,10 +6795,10 @@
         <v>81</v>
       </c>
       <c r="K16" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L16" s="17" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M16" t="b">
         <v>0</v>
@@ -6810,13 +6825,13 @@
         <v>10</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C17" s="14" t="s">
         <v>124</v>
       </c>
       <c r="D17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E17" s="14" t="s">
         <v>92</v>
@@ -6824,11 +6839,11 @@
       <c r="F17" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="G17" s="119">
+      <c r="G17" s="117">
         <v>2020</v>
       </c>
       <c r="H17" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I17" s="14" t="str">
         <f t="shared" si="0"/>
@@ -6838,10 +6853,10 @@
         <v>73</v>
       </c>
       <c r="K17" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L17" s="17" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="M17" t="b">
         <v>0</v>
@@ -6868,13 +6883,13 @@
         <v>11</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C18" s="14" t="s">
         <v>124</v>
       </c>
       <c r="D18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E18" s="14" t="s">
         <v>92</v>
@@ -6882,11 +6897,11 @@
       <c r="F18" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="G18" s="119">
+      <c r="G18" s="117">
         <v>2020</v>
       </c>
       <c r="H18" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I18" s="14" t="str">
         <f t="shared" si="0"/>
@@ -6896,10 +6911,10 @@
         <v>73</v>
       </c>
       <c r="K18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L18" s="17" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="M18" t="b">
         <v>0</v>
@@ -6926,13 +6941,13 @@
         <v>12</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C19" s="14" t="s">
         <v>124</v>
       </c>
       <c r="D19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E19" s="14" t="s">
         <v>92</v>
@@ -6940,11 +6955,11 @@
       <c r="F19" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="G19" s="119">
+      <c r="G19" s="117">
         <v>2020</v>
       </c>
       <c r="H19" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I19" s="14" t="str">
         <f t="shared" si="0"/>
@@ -6954,10 +6969,10 @@
         <v>73</v>
       </c>
       <c r="K19" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L19" s="17" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="M19" t="b">
         <v>0</v>
@@ -6984,13 +6999,13 @@
         <v>13</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C20" s="14" t="s">
         <v>113</v>
       </c>
       <c r="D20" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E20" s="14" t="s">
         <v>92</v>
@@ -6998,11 +7013,11 @@
       <c r="F20" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="G20" s="119">
+      <c r="G20" s="117">
         <v>2020</v>
       </c>
       <c r="H20" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I20" s="14" t="str">
         <f t="shared" si="0"/>
@@ -7012,10 +7027,10 @@
         <v>73</v>
       </c>
       <c r="K20" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L20" s="17" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="M20" t="b">
         <v>0</v>
@@ -7042,13 +7057,13 @@
         <v>14</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C21" s="14" t="s">
         <v>113</v>
       </c>
       <c r="D21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E21" s="14" t="s">
         <v>92</v>
@@ -7056,11 +7071,11 @@
       <c r="F21" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="G21" s="119">
+      <c r="G21" s="117">
         <v>2020</v>
       </c>
       <c r="H21" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I21" s="14" t="str">
         <f t="shared" si="0"/>
@@ -7070,10 +7085,10 @@
         <v>73</v>
       </c>
       <c r="K21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L21" s="17" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="M21" t="b">
         <v>0</v>
@@ -7100,13 +7115,13 @@
         <v>15</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C22" s="14" t="s">
         <v>113</v>
       </c>
       <c r="D22" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E22" s="14" t="s">
         <v>92</v>
@@ -7114,11 +7129,11 @@
       <c r="F22" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="G22" s="119">
+      <c r="G22" s="117">
         <v>2020</v>
       </c>
       <c r="H22" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I22" s="14" t="str">
         <f t="shared" si="0"/>
@@ -7128,10 +7143,10 @@
         <v>73</v>
       </c>
       <c r="K22" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L22" s="17" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="M22" t="b">
         <v>0</v>
@@ -7158,13 +7173,13 @@
         <v>16</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D23" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E23" s="14" t="s">
         <v>92</v>
@@ -7172,11 +7187,11 @@
       <c r="F23" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="G23" s="119">
+      <c r="G23" s="117">
         <v>2020</v>
       </c>
       <c r="H23" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I23" s="14" t="str">
         <f t="shared" si="0"/>
@@ -7186,10 +7201,10 @@
         <v>73</v>
       </c>
       <c r="K23" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L23" s="17" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="M23" t="b">
         <v>0</v>
@@ -7216,13 +7231,13 @@
         <v>17</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D24" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E24" s="14" t="s">
         <v>92</v>
@@ -7230,11 +7245,11 @@
       <c r="F24" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="G24" s="119">
+      <c r="G24" s="117">
         <v>2020</v>
       </c>
       <c r="H24" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I24" s="14" t="str">
         <f t="shared" si="0"/>
@@ -7244,10 +7259,10 @@
         <v>73</v>
       </c>
       <c r="K24" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L24" s="17" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="M24" t="b">
         <v>0</v>
@@ -7274,13 +7289,13 @@
         <v>18</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D25" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E25" s="14" t="s">
         <v>92</v>
@@ -7288,11 +7303,11 @@
       <c r="F25" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="G25" s="119">
+      <c r="G25" s="117">
         <v>2020</v>
       </c>
       <c r="H25" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I25" s="14" t="str">
         <f t="shared" si="0"/>
@@ -7302,10 +7317,10 @@
         <v>73</v>
       </c>
       <c r="K25" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L25" s="17" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="M25" t="b">
         <v>0</v>

</xml_diff>